<commit_message>
clean up comparison table
</commit_message>
<xml_diff>
--- a/joss_paper/tables.xlsx
+++ b/joss_paper/tables.xlsx
@@ -2,19 +2,22 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28109"/>
-  <workbookPr/>
+  <workbookPr checkCompatibility="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arthur_at_sinai/gitOnMyLaptopLocal/wc_dev_repos/de_sim/joss_paper/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="19420" yWindow="8080" windowWidth="18040" windowHeight="12780" activeTab="1"/>
+    <workbookView xWindow="1080" yWindow="2080" windowWidth="26660" windowHeight="13760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Performance" sheetId="1" r:id="rId1"/>
     <sheet name="Comparison with DES tools" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'Comparison with DES tools'!$B$2:$J$8</definedName>
+  </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -28,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="33">
   <si>
     <t>Run time (s)</t>
   </si>
@@ -69,33 +72,15 @@
     <t>Std dev</t>
   </si>
   <si>
-    <t>Tool</t>
-  </si>
-  <si>
     <t>DE-Sim</t>
   </si>
   <si>
-    <t>Language</t>
-  </si>
-  <si>
-    <t>License</t>
-  </si>
-  <si>
-    <t>GUI interface</t>
-  </si>
-  <si>
     <t>Space-time diagrams</t>
   </si>
   <si>
     <t>SimPy</t>
   </si>
   <si>
-    <t>Process-based framework</t>
-  </si>
-  <si>
-    <t>Object-oriented simulation</t>
-  </si>
-  <si>
     <t>SystemC</t>
   </si>
   <si>
@@ -114,22 +99,58 @@
     <t>Open-source</t>
   </si>
   <si>
-    <t>Proprietary</t>
-  </si>
-  <si>
     <t>Year released</t>
   </si>
   <si>
-    <t>Hardware simulator</t>
-  </si>
-  <si>
-    <t>Domain</t>
-  </si>
-  <si>
     <t>General purpose object-oriented simulation</t>
   </si>
   <si>
-    <t>Yes</t>
+    <t>✓</t>
+  </si>
+  <si>
+    <t>Digital hardware</t>
+  </si>
+  <si>
+    <t>General purpose process-based framework</t>
+  </si>
+  <si>
+    <t>WSC citations</t>
+  </si>
+  <si>
+    <t>C++</t>
+  </si>
+  <si>
+    <t>Business processes</t>
+  </si>
+  <si>
+    <t>Simulation tool</t>
+  </si>
+  <si>
+    <t>Communications networks</t>
+  </si>
+  <si>
+    <t>MATLAB</t>
+  </si>
+  <si>
+    <t>Parallelizable</t>
+  </si>
+  <si>
+    <t>Application domain</t>
+  </si>
+  <si>
+    <t>Complex, data-intensive models</t>
+  </si>
+  <si>
+    <t>GUI model builder</t>
+  </si>
+  <si>
+    <t>Visual Logic</t>
+  </si>
+  <si>
+    <t>Modeling language</t>
+  </si>
+  <si>
+    <t>Object-oriented models</t>
   </si>
 </sst>
 </file>
@@ -140,7 +161,7 @@
     <numFmt numFmtId="164" formatCode="#,##0.00_ "/>
     <numFmt numFmtId="165" formatCode="#,##0_ "/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -173,6 +194,11 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -182,7 +208,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -190,13 +216,55 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -218,8 +286,56 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="distributed" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="distributed" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="distributed" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -678,112 +794,217 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H7"/>
+  <sheetPr enableFormatConditionsCalculation="0">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B1:N8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
+      <selection activeCell="J8" sqref="B2:J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="21.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" customWidth="1"/>
+    <col min="1" max="1" width="4.1640625" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" customWidth="1"/>
+    <col min="6" max="6" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5" customWidth="1"/>
+    <col min="9" max="9" width="8.1640625" customWidth="1"/>
+    <col min="10" max="10" width="7.83203125" customWidth="1"/>
+    <col min="11" max="11" width="8" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="2:11" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:11" ht="46" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" ht="30" x14ac:dyDescent="0.2">
+      <c r="B3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="C3" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="10"/>
+      <c r="G3" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="21">
+        <v>2020</v>
+      </c>
+      <c r="K3" s="10"/>
+    </row>
+    <row r="4" spans="2:11" ht="45" x14ac:dyDescent="0.2">
+      <c r="B4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="9"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="9"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="22">
+        <v>2002</v>
+      </c>
+      <c r="K4" s="7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B5" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="7"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" s="22">
+        <v>2000</v>
+      </c>
+      <c r="K5" s="7">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
+      <c r="B6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="9"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="22">
+        <v>1994</v>
+      </c>
+      <c r="K6" s="7">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" ht="45" x14ac:dyDescent="0.2">
+      <c r="B7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="J7" s="22">
+        <v>1971</v>
+      </c>
+      <c r="K7" s="7">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" ht="31" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="30" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="6" t="s">
+      <c r="D8" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="C2">
-        <v>2020</v>
-      </c>
-      <c r="D2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="E8" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="F6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" t="s">
-        <v>21</v>
+      <c r="F8" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="17"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="23">
+        <v>2007</v>
+      </c>
+      <c r="K8" s="15">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
more on existing DES tools
</commit_message>
<xml_diff>
--- a/joss_paper/tables.xlsx
+++ b/joss_paper/tables.xlsx
@@ -9,15 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-51000" yWindow="25960" windowWidth="24440" windowHeight="11540" activeTab="1"/>
+    <workbookView xWindow="2580" yWindow="9920" windowWidth="21540" windowHeight="11640"/>
   </bookViews>
   <sheets>
     <sheet name="Performance" sheetId="1" r:id="rId1"/>
-    <sheet name="Comparison with DES tools" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'Comparison with DES tools'!$B$2:$J$8</definedName>
-  </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -31,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
     <t>Run time (s)</t>
   </si>
@@ -71,87 +67,6 @@
   <si>
     <t>Std dev</t>
   </si>
-  <si>
-    <t>DE-Sim</t>
-  </si>
-  <si>
-    <t>Space-time diagrams</t>
-  </si>
-  <si>
-    <t>SimPy</t>
-  </si>
-  <si>
-    <t>SystemC</t>
-  </si>
-  <si>
-    <t>SIMUL8</t>
-  </si>
-  <si>
-    <t>SIMSCRIPT III</t>
-  </si>
-  <si>
-    <t>SimEvents</t>
-  </si>
-  <si>
-    <t>Python</t>
-  </si>
-  <si>
-    <t>Open-source</t>
-  </si>
-  <si>
-    <t>Year released</t>
-  </si>
-  <si>
-    <t>General purpose object-oriented simulation</t>
-  </si>
-  <si>
-    <t>✓</t>
-  </si>
-  <si>
-    <t>Digital hardware</t>
-  </si>
-  <si>
-    <t>General purpose process-based framework</t>
-  </si>
-  <si>
-    <t>C++</t>
-  </si>
-  <si>
-    <t>Business processes</t>
-  </si>
-  <si>
-    <t>Simulation tool</t>
-  </si>
-  <si>
-    <t>Communications networks</t>
-  </si>
-  <si>
-    <t>MATLAB</t>
-  </si>
-  <si>
-    <t>Parallelizable</t>
-  </si>
-  <si>
-    <t>Application domain</t>
-  </si>
-  <si>
-    <t>Complex, data-intensive models</t>
-  </si>
-  <si>
-    <t>GUI model builder</t>
-  </si>
-  <si>
-    <t>Visual Logic</t>
-  </si>
-  <si>
-    <t>Modeling language</t>
-  </si>
-  <si>
-    <t>Object-oriented models</t>
-  </si>
-  <si>
-    <t>WSC publications</t>
-  </si>
 </sst>
 </file>
 
@@ -161,7 +76,7 @@
     <numFmt numFmtId="164" formatCode="#,##0.00_ "/>
     <numFmt numFmtId="165" formatCode="#,##0_ "/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -187,81 +102,21 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2" tint="-9.9948118533890809E-2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="5">
+  <borders count="1">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -270,7 +125,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -288,63 +143,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="distributed" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="distributed" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="distributed" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -620,7 +418,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
@@ -799,221 +597,4 @@
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="B1:N8"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="4.1640625" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10" customWidth="1"/>
-    <col min="6" max="6" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.5" customWidth="1"/>
-    <col min="9" max="9" width="8.1640625" customWidth="1"/>
-    <col min="10" max="10" width="7.83203125" customWidth="1"/>
-    <col min="11" max="11" width="11" hidden="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:11" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:11" ht="46" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="I2" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="J2" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="K2" s="12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="2:11" ht="30" x14ac:dyDescent="0.2">
-      <c r="B3" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="21" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" s="20"/>
-      <c r="G3" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" s="23" t="s">
-        <v>17</v>
-      </c>
-      <c r="J3" s="24">
-        <v>2020</v>
-      </c>
-      <c r="K3" s="10"/>
-    </row>
-    <row r="4" spans="2:11" ht="45" x14ac:dyDescent="0.2">
-      <c r="B4" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="9"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="J4" s="18">
-        <v>2002</v>
-      </c>
-      <c r="K4" s="7">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B5" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="7"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="J5" s="18">
-        <v>2000</v>
-      </c>
-      <c r="K5" s="7">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.2">
-      <c r="B6" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" s="9"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="18">
-        <v>1994</v>
-      </c>
-      <c r="K6" s="7">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="7" spans="2:11" ht="45" x14ac:dyDescent="0.2">
-      <c r="B7" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="18">
-        <v>1971</v>
-      </c>
-      <c r="K7" s="7">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="8" spans="2:11" ht="31" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="F8" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" s="15"/>
-      <c r="H8" s="13"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="19">
-        <v>2007</v>
-      </c>
-      <c r="K8" s="13">
-        <v>24</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
-</worksheet>
 </file>
</xml_diff>